<commit_message>
Stworzenie bug report dla jedynego FAIL w TC_08
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\portfolio\Tester manualny - junior\OpenWeatherMapAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EF1115-8F35-4CD8-BA5D-E34C2F123472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC5AFA0-8172-4DF0-8417-A9EDE0882BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -246,10 +246,10 @@
     <t>Status 400, Informacja o niepoprawnych danych na wejściu(wyspecyfikowanie których)</t>
   </si>
   <si>
-    <t>Status 200, nie ma określonych wszytskich danych, które są niepoprawne</t>
-  </si>
-  <si>
     <t>FAIL</t>
+  </si>
+  <si>
+    <t>Status 400, nie ma określonych wszytskich danych, które są niepoprawne</t>
   </si>
 </sst>
 </file>
@@ -588,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="A1:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1040,8 +1040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A65C0EF6-C0A4-41AA-AAA8-F3209CFBB647}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1197,10 +1197,10 @@
         <v>62</v>
       </c>
       <c r="J4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>